<commit_message>
Add 6.Issue Report for Testcase[ST16_CGOET].xlsx
</commit_message>
<xml_diff>
--- a/1.TestCase[SW]/TestCase(ST16_CGOET).xlsx
+++ b/1.TestCase[SW]/TestCase(ST16_CGOET).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="29040" windowHeight="16440" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="29040" windowHeight="16440" tabRatio="447" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="1.Result Status" sheetId="1" r:id="rId1"/>
@@ -12,9 +12,10 @@
     <sheet name="3.Firmware Version" sheetId="3" r:id="rId3"/>
     <sheet name="4.Update History" sheetId="2" r:id="rId4"/>
     <sheet name="5.Testcase_CGOET" sheetId="7" r:id="rId5"/>
-    <sheet name="6.Bug Report" sheetId="5" r:id="rId6"/>
+    <sheet name="6.Issue Report" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="125725" concurrentCalc="0"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -23,107 +24,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>作者</author>
-  </authors>
-  <commentList>
-    <comment ref="G14" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="ＭＳ Ｐゴシック"/>
-            <charset val="128"/>
-          </rPr>
-          <t>丁正</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>龙</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="ＭＳ Ｐゴシック"/>
-            <charset val="128"/>
-          </rPr>
-          <t>:     
-功能及用</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>户</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="ＭＳ Ｐゴシック"/>
-            <charset val="128"/>
-          </rPr>
-          <t>体</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>验鉴别</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="ＭＳ Ｐゴシック"/>
-            <charset val="128"/>
-          </rPr>
-          <t>待</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>确认</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="139">
   <si>
     <t>Passed</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -189,10 +91,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Bug ID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Test Result Status</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -202,26 +100,6 @@
   </si>
   <si>
     <t>Firmware Version</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bug Summary</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bug Description</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Bug Rank </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bug Status</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bug Reporter</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1085,104 +963,6 @@
     <t>CGOET_设置拍摄_AutoCalibration</t>
     <rPh sb="6" eb="7">
       <t>she zhi</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.切换Auto Calibration开关，检查红外拍摄温度状态变化；</t>
-    <rPh sb="2" eb="3">
-      <t>qie huan</t>
-    </rPh>
-    <rPh sb="20" eb="21">
-      <t>kai guan</t>
-    </rPh>
-    <rPh sb="23" eb="24">
-      <t>jian cha</t>
-    </rPh>
-    <rPh sb="25" eb="26">
-      <t>hong wai</t>
-    </rPh>
-    <rPh sb="27" eb="28">
-      <t>pai she</t>
-    </rPh>
-    <rPh sb="29" eb="30">
-      <t>wen du zhi</t>
-    </rPh>
-    <rPh sb="31" eb="32">
-      <t>zhuang tai</t>
-    </rPh>
-    <rPh sb="33" eb="34">
-      <t>bian hua</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.当Auto Calibration开关打开时，红外拍摄自动校准拍摄温度值；当Auto Calibration开关关闭时，红外拍摄将不会自动校准拍摄温度值；</t>
-    <rPh sb="2" eb="3">
-      <t>dang</t>
-    </rPh>
-    <rPh sb="19" eb="20">
-      <t>kai guan</t>
-    </rPh>
-    <rPh sb="21" eb="22">
-      <t>da kai</t>
-    </rPh>
-    <rPh sb="23" eb="24">
-      <t>shi hou</t>
-    </rPh>
-    <rPh sb="25" eb="26">
-      <t>hong wai</t>
-    </rPh>
-    <rPh sb="27" eb="28">
-      <t>pai she</t>
-    </rPh>
-    <rPh sb="29" eb="30">
-      <t>zi dong</t>
-    </rPh>
-    <rPh sb="31" eb="32">
-      <t>jiao zhun</t>
-    </rPh>
-    <rPh sb="33" eb="34">
-      <t>pai she</t>
-    </rPh>
-    <rPh sb="35" eb="36">
-      <t>wen du zhi</t>
-    </rPh>
-    <rPh sb="39" eb="40">
-      <t>dang</t>
-    </rPh>
-    <rPh sb="56" eb="57">
-      <t>kai guan</t>
-    </rPh>
-    <rPh sb="58" eb="59">
-      <t>guan bi</t>
-    </rPh>
-    <rPh sb="60" eb="61">
-      <t>shi hou</t>
-    </rPh>
-    <rPh sb="62" eb="63">
-      <t>hong wai</t>
-    </rPh>
-    <rPh sb="64" eb="65">
-      <t>pai she</t>
-    </rPh>
-    <rPh sb="66" eb="67">
-      <t>jiang</t>
-    </rPh>
-    <rPh sb="67" eb="68">
-      <t>bu hui</t>
-    </rPh>
-    <rPh sb="69" eb="70">
-      <t>zi dong</t>
-    </rPh>
-    <rPh sb="71" eb="72">
-      <t>jiao zhun</t>
-    </rPh>
-    <rPh sb="73" eb="74">
-      <t>pai she</t>
-    </rPh>
-    <rPh sb="75" eb="76">
-      <t>wen du zhi</t>
     </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -3192,13 +2972,7 @@
       <t>ji</t>
     </rPh>
     <rPh sb="97" eb="98">
-      <t>yun tai</t>
-    </rPh>
-    <rPh sb="237" eb="238">
-      <t>yu lan</t>
-    </rPh>
-    <rPh sb="239" eb="240">
-      <t>pai s</t>
+      <t>yun taiyu lanpai s</t>
     </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -3244,13 +3018,7 @@
       <t>ji</t>
     </rPh>
     <rPh sb="140" eb="141">
-      <t>yun tai</t>
-    </rPh>
-    <rPh sb="280" eb="281">
-      <t>she zhyi</t>
-    </rPh>
-    <rPh sb="282" eb="283">
-      <t>pai she</t>
+      <t>yun taishe zhyipai she</t>
     </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -3333,13 +3101,7 @@
       <t>ji</t>
     </rPh>
     <rPh sb="117" eb="118">
-      <t>yun tai</t>
-    </rPh>
-    <rPh sb="257" eb="258">
-      <t>she zhyi</t>
-    </rPh>
-    <rPh sb="259" eb="260">
-      <t>pai she</t>
+      <t>yun taishe zhyipai she</t>
     </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -3373,13 +3135,7 @@
       <t>yun tai</t>
     </rPh>
     <rPh sb="178" eb="179">
-      <t>ji</t>
-    </rPh>
-    <rPh sb="267" eb="268">
-      <t>she zhyi</t>
-    </rPh>
-    <rPh sb="269" eb="270">
-      <t>pai she</t>
+      <t>jishe zhyipai she</t>
     </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -3425,13 +3181,7 @@
       <t>ji</t>
     </rPh>
     <rPh sb="140" eb="141">
-      <t>yun tai</t>
-    </rPh>
-    <rPh sb="280" eb="281">
-      <t>she zhyi</t>
-    </rPh>
-    <rPh sb="282" eb="283">
-      <t>pai she</t>
+      <t>yun taishe zhyipai she</t>
     </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -3519,19 +3269,334 @@
       <t>zhong</t>
     </rPh>
     <rPh sb="186" eb="187">
-      <t>wen du</t>
-    </rPh>
-    <rPh sb="188" eb="189">
-      <t>dan wei</t>
-    </rPh>
-    <rPh sb="190" eb="191">
-      <t>xian shi</t>
-    </rPh>
-    <rPh sb="192" eb="193">
-      <t>xin xi</t>
-    </rPh>
-    <rPh sb="194" eb="195">
+      <t>wen dudan weixian shixin xibian hua</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ST16-32</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
+  </si>
+  <si>
+    <t>Low</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Resolved</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>丁正龙</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fixed，will double confirm with next version.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Priority</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reporter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Summary</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bug</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Issue ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Resolution</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fixed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>st16_system_v03.01.b22</t>
+  </si>
+  <si>
+    <t>Environment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Due Date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Affect Version/s:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[ST16]C-GOET云台移除SD Card时图传界面状态显示异常(0.00G)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[ST16]Camera Select中重复选择C-GOET提示信息有误(见附图)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">System Version: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">st16_system_v03.01.b22(BuildDate:2016-07-06) 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Transmitter Version: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">st16_tx_v00.19 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Radio Version: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">st16_rf_v01.09 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">FlightMode Version: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>st16_app_v01.00.18</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I.前置条件： 
+  刷b20测试版本Firmware 
+  \\192.168.6.247\smartteam-release\ST16\dailybuild4test\st16_system_v03.01.b20_2016-07-01 
+II.复现步骤： 
+  1.刷机后进入系统，单击进入FlightMode App； 
+  2.在System Settings-&gt;Bind下绑定Camera； 
+  3.在System Settings-&gt;Camera Select切换Camera为C-GOET； 
+  4.返回FlightMode主界面，待图传正常时再次进入Camera Select选择C-GOET进行切换； 
+  5.检查Camera Select按钮提示信息是否正常，检查图传界面是否正常； 
+III.预期结果： 
+  1.重新切换Camera后单击Select后提示信息应为"Setup Complete!"且图传界面正常； 
+IV.实际结果： 
+  1.重新切换Camera单击Select后 弹出"Connect to the Flight System..."界面，同时Set Status界面提示信息为"Set failure!",但是图传信息正常； 
+V.附加信息： 
+  1.复现率：100%； 
+  2.比较验证不同类型云台(C-GO3,C-GO3-PRO,C-GOET),目前该现象仅出现在C-GOET上；</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I.前置条件： 
+  刷b22测试版本Firmware 
+\\192.168.6.247\smartteam- release\ST16\dailybuild4test\st16_system_v03.01.b22_2016-07-26 
+II.复现步骤： 
+  1.刷机后进入系统，单击进入FlightMode App； 
+  2.Bind云台C-GOET并插入储量未满SD Card； 
+  3.检查图传界面SD Card状态信息； 
+  4.移除云台C-GOET的SD Card； 
+  5.检查图传界面SD Card状态变化信息； 
+III.预期结果： 
+  1.插入SD Card图传界面正确显示其储量信息； 
+  2.移除SD Card图传界面状态变为Not Detected； 
+IV.实际结果： 
+  1.插入SD Card图传界面正确显示其储量信息； 
+  2.移除SD Card图传界面状态变为0.00G； 
+V.附加信息： 
+  1.复现率：100%； 
+  2.目前该现象出现在C-GOET，不出现在C-GO3-Pro；</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[ST16]C-GOET中Auto Calibration切换功能及状态异常(见附图)</t>
+  </si>
+  <si>
+    <t>Medium</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I.前置条件： 
+  刷b22测试版本Firmware 
+  \\192.168.6.247\smartteam-release\ST16\dailybuild4test\st16_system_v03.01.b22_2016-07-26 
+II.复现步骤： 
+  1.刷机后进入系统，单击进入FlightMode App； 
+  2.在System Settings-&gt;Bind下绑定飞机及云台(C-GOET)； 
+  3.在图传界面Camera Settings-&gt;Auto Calibration执行切换操作； 
+  4.检查Auto Calibration切换后状态及页面提示信息； 
+III预期结果： 
+  1.Auto Calibration按钮可以在On与Off之间切换，同时不出现Error信息； 
+IV.实际结果： 
+  1.单击Auto Calibration按钮后，On与Off之间没有发生切换，同时页面出现'Auto Calibrate Set Fail'的Error信息，但单击Camera Settings按钮再次打开时Auto Calibration状态发生改变； 
+V.附加信息： 
+  1.复现率：100%；</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unresolved</t>
+  </si>
+  <si>
+    <t>Open</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ST16-27</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ST16-29</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.切换Auto Calibration开关，检查切换功能及状态信息；</t>
+    <rPh sb="2" eb="3">
+      <t>qie huan</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>kai guan</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>jian cha</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>hong wai</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>pai she</t>
+    </rPh>
+    <rPh sb="29" eb="30">
+      <t>wen du zhi</t>
+    </rPh>
+    <rPh sb="31" eb="32">
+      <t>zhuang tai</t>
+    </rPh>
+    <rPh sb="33" eb="34">
       <t>bian hua</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.Auto Calibration可以在On与Off之间进行切换，同时没有任何Error信息；</t>
+    <rPh sb="2" eb="3">
+      <t>dang</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>kai guan</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>da kai</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>shi hou</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>hong wai</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>pai she</t>
+    </rPh>
+    <rPh sb="29" eb="30">
+      <t>zi dong</t>
+    </rPh>
+    <rPh sb="31" eb="32">
+      <t>jiao zhun</t>
+    </rPh>
+    <rPh sb="33" eb="34">
+      <t>pai she</t>
+    </rPh>
+    <rPh sb="35" eb="36">
+      <t>wen du zhi</t>
+    </rPh>
+    <rPh sb="39" eb="40">
+      <t>dangkai guanguan bishi houhong waipai shejiangbu huizi dongjiao zhunpai shewen du zhi</t>
     </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -3607,22 +3672,23 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color indexed="81"/>
-      <name val="ＭＳ Ｐゴシック"/>
-      <charset val="128"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color indexed="81"/>
+      <color theme="10"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3669,12 +3735,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF0070C0"/>
         <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -3840,7 +3900,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3862,8 +3922,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3915,9 +3979,6 @@
     <xf numFmtId="0" fontId="6" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -3934,6 +3995,24 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="7" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3994,11 +4073,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="8">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="7" builtinId="8"/>
     <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
@@ -4352,13 +4432,13 @@
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5"/>
   <sheetData>
     <row r="9" spans="8:12">
-      <c r="H9" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="I9" s="24"/>
-      <c r="J9" s="24"/>
-      <c r="K9" s="24"/>
-      <c r="L9" s="24"/>
+      <c r="H9" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="29"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="29"/>
+      <c r="L9" s="29"/>
     </row>
     <row r="10" spans="8:12" ht="15">
       <c r="H10" s="1" t="s">
@@ -4391,51 +4471,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:Q4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5"/>
   <sheetData>
     <row r="3" spans="1:17">
-      <c r="A3" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
-      <c r="M3" s="26"/>
-      <c r="N3" s="26"/>
-      <c r="O3" s="26"/>
-      <c r="P3" s="26"/>
-      <c r="Q3" s="27"/>
+      <c r="A3" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="31"/>
+      <c r="O3" s="31"/>
+      <c r="P3" s="31"/>
+      <c r="Q3" s="32"/>
     </row>
     <row r="4" spans="1:17">
-      <c r="A4" s="28"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="29"/>
-      <c r="O4" s="29"/>
-      <c r="P4" s="29"/>
-      <c r="Q4" s="30"/>
+      <c r="A4" s="33"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="34"/>
+      <c r="L4" s="34"/>
+      <c r="M4" s="34"/>
+      <c r="N4" s="34"/>
+      <c r="O4" s="34"/>
+      <c r="P4" s="34"/>
+      <c r="Q4" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4468,7 +4548,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>6</v>
@@ -4479,13 +4559,13 @@
     </row>
     <row r="2" spans="1:4" ht="168.95" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
+        <v>18</v>
+      </c>
+      <c r="B2" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4515,7 +4595,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="5" customFormat="1">
       <c r="A1" s="12" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -4541,13 +4621,13 @@
         <v>11</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="F2" s="13" t="s">
         <v>15</v>
@@ -4634,8 +4714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="13.5"/>
@@ -4652,59 +4732,59 @@
   <sheetData>
     <row r="1" spans="1:12" ht="27">
       <c r="A1" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="45" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="46"/>
+      <c r="D1" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="I1" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="16" t="s">
+      <c r="J1" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="K1" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="L1" s="16" t="s">
         <v>31</v>
-      </c>
-      <c r="G1" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="H1" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="I1" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="J1" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="K1" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="L1" s="16" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="121.5">
       <c r="A2" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="22" t="s">
-        <v>103</v>
+        <v>35</v>
+      </c>
+      <c r="B2" s="47" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="47"/>
+      <c r="D2" s="21" t="s">
+        <v>95</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="F2" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="G2" s="20" t="s">
-        <v>95</v>
+        <v>32</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>87</v>
       </c>
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
@@ -4714,23 +4794,23 @@
     </row>
     <row r="3" spans="1:12" ht="121.5">
       <c r="A3" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="23" t="s">
-        <v>104</v>
+        <v>34</v>
+      </c>
+      <c r="B3" s="43" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="43"/>
+      <c r="D3" s="22" t="s">
+        <v>96</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
@@ -4740,23 +4820,23 @@
     </row>
     <row r="4" spans="1:12" ht="135">
       <c r="A4" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" s="38" t="s">
-        <v>76</v>
-      </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="23" t="s">
-        <v>104</v>
+        <v>39</v>
+      </c>
+      <c r="B4" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="43"/>
+      <c r="D4" s="22" t="s">
+        <v>96</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="G4" s="23" t="s">
-        <v>105</v>
+        <v>40</v>
+      </c>
+      <c r="G4" s="22" t="s">
+        <v>97</v>
       </c>
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
@@ -4766,23 +4846,23 @@
     </row>
     <row r="5" spans="1:12" ht="121.5">
       <c r="A5" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="38" t="s">
-        <v>77</v>
-      </c>
-      <c r="C5" s="38"/>
-      <c r="D5" s="23" t="s">
-        <v>104</v>
+        <v>38</v>
+      </c>
+      <c r="B5" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="43"/>
+      <c r="D5" s="22" t="s">
+        <v>96</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="G5" s="20" t="s">
-        <v>96</v>
+        <v>32</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>88</v>
       </c>
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
@@ -4791,24 +4871,24 @@
       <c r="L5" s="14"/>
     </row>
     <row r="6" spans="1:12" ht="121.5">
-      <c r="A6" s="39" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="38"/>
-      <c r="D6" s="23" t="s">
-        <v>104</v>
+      <c r="A6" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="43"/>
+      <c r="D6" s="22" t="s">
+        <v>96</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
@@ -4817,22 +4897,22 @@
       <c r="L6" s="14"/>
     </row>
     <row r="7" spans="1:12" ht="148.5">
-      <c r="A7" s="39"/>
-      <c r="B7" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="23" t="s">
-        <v>106</v>
+      <c r="A7" s="44"/>
+      <c r="B7" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="43"/>
+      <c r="D7" s="22" t="s">
+        <v>98</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="G7" s="18" t="s">
-        <v>85</v>
+        <v>32</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>77</v>
       </c>
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
@@ -4841,325 +4921,325 @@
       <c r="L7" s="14"/>
     </row>
     <row r="8" spans="1:12" ht="121.5">
-      <c r="A8" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="C8" s="37"/>
-      <c r="D8" s="23" t="s">
-        <v>104</v>
-      </c>
-      <c r="E8" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="G8" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
+      <c r="A8" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="42"/>
+      <c r="D8" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
     </row>
     <row r="9" spans="1:12" ht="148.5">
-      <c r="A9" s="34"/>
-      <c r="B9" s="36" t="s">
-        <v>90</v>
-      </c>
-      <c r="C9" s="37"/>
-      <c r="D9" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="G9" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
+      <c r="A9" s="39"/>
+      <c r="B9" s="41" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" s="42"/>
+      <c r="D9" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="G9" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
     </row>
     <row r="10" spans="1:12" ht="148.5">
-      <c r="A10" s="34"/>
-      <c r="B10" s="36" t="s">
+      <c r="A10" s="39"/>
+      <c r="B10" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" s="42"/>
+      <c r="D10" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="C10" s="37"/>
-      <c r="D10" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="F10" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="G10" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
+      <c r="G10" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
     </row>
     <row r="11" spans="1:12" ht="121.5">
-      <c r="A11" s="34"/>
-      <c r="B11" s="36" t="s">
-        <v>57</v>
-      </c>
-      <c r="C11" s="37"/>
-      <c r="D11" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="F11" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="G11" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="19"/>
+      <c r="A11" s="39"/>
+      <c r="B11" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="42"/>
+      <c r="D11" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
     </row>
     <row r="12" spans="1:12" ht="121.5">
-      <c r="A12" s="34"/>
-      <c r="B12" s="36" t="s">
-        <v>58</v>
-      </c>
-      <c r="C12" s="37"/>
-      <c r="D12" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="E12" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="F12" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="G12" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19"/>
+      <c r="A12" s="39"/>
+      <c r="B12" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="42"/>
+      <c r="D12" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
     </row>
     <row r="13" spans="1:12" ht="121.5">
-      <c r="A13" s="34"/>
-      <c r="B13" s="36" t="s">
-        <v>62</v>
-      </c>
-      <c r="C13" s="37"/>
-      <c r="D13" s="23" t="s">
-        <v>110</v>
-      </c>
-      <c r="E13" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="F13" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="G13" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="19"/>
-      <c r="K13" s="19"/>
-      <c r="L13" s="19"/>
+      <c r="A13" s="39"/>
+      <c r="B13" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="42"/>
+      <c r="D13" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
     </row>
     <row r="14" spans="1:12" ht="121.5">
-      <c r="A14" s="34"/>
-      <c r="B14" s="36" t="s">
-        <v>65</v>
-      </c>
-      <c r="C14" s="37"/>
-      <c r="D14" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="F14" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="G14" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="19"/>
-      <c r="K14" s="19"/>
-      <c r="L14" s="19"/>
+      <c r="A14" s="39"/>
+      <c r="B14" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="42"/>
+      <c r="D14" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="G14" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
     </row>
     <row r="15" spans="1:12" ht="121.5">
-      <c r="A15" s="34"/>
-      <c r="B15" s="36" t="s">
-        <v>68</v>
-      </c>
-      <c r="C15" s="37"/>
-      <c r="D15" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="F15" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="G15" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="19"/>
-      <c r="K15" s="19"/>
-      <c r="L15" s="19"/>
+      <c r="A15" s="39"/>
+      <c r="B15" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="42"/>
+      <c r="D15" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="G15" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
     </row>
     <row r="16" spans="1:12" ht="148.5">
-      <c r="A16" s="34"/>
-      <c r="B16" s="36" t="s">
-        <v>70</v>
-      </c>
-      <c r="C16" s="37"/>
-      <c r="D16" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="E16" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="F16" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="G16" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="19"/>
-      <c r="K16" s="19"/>
-      <c r="L16" s="19"/>
+      <c r="A16" s="39"/>
+      <c r="B16" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="42"/>
+      <c r="D16" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="G16" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="18"/>
     </row>
     <row r="17" spans="1:12" ht="121.5">
-      <c r="A17" s="34"/>
-      <c r="B17" s="36" t="s">
-        <v>72</v>
-      </c>
-      <c r="C17" s="37"/>
-      <c r="D17" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="E17" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="F17" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="G17" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19"/>
-      <c r="L17" s="19"/>
+      <c r="A17" s="39"/>
+      <c r="B17" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="42"/>
+      <c r="D17" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="G17" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
     </row>
     <row r="18" spans="1:12" ht="121.5">
-      <c r="A18" s="34"/>
-      <c r="B18" s="36" t="s">
-        <v>80</v>
-      </c>
-      <c r="C18" s="37"/>
-      <c r="D18" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="E18" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="F18" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="G18" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="19"/>
+      <c r="A18" s="39"/>
+      <c r="B18" s="41" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" s="42"/>
+      <c r="D18" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="G18" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="18"/>
     </row>
     <row r="19" spans="1:12" ht="121.5">
-      <c r="A19" s="34"/>
-      <c r="B19" s="38" t="s">
-        <v>81</v>
-      </c>
-      <c r="C19" s="38"/>
-      <c r="D19" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="E19" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="F19" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="G19" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
+      <c r="A19" s="39"/>
+      <c r="B19" s="43" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="43"/>
+      <c r="D19" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="G19" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="19"/>
+      <c r="L19" s="19"/>
     </row>
     <row r="20" spans="1:12" ht="121.5">
-      <c r="A20" s="35"/>
-      <c r="B20" s="36" t="s">
-        <v>86</v>
-      </c>
-      <c r="C20" s="37"/>
-      <c r="D20" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="E20" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="F20" s="23" t="s">
-        <v>112</v>
-      </c>
-      <c r="G20" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="H20" s="20"/>
-      <c r="I20" s="20"/>
-      <c r="J20" s="20"/>
-      <c r="K20" s="20"/>
-      <c r="L20" s="20"/>
+      <c r="A20" s="40"/>
+      <c r="B20" s="41" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" s="42"/>
+      <c r="D20" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="G20" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="19"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="19"/>
     </row>
     <row r="24" spans="1:12">
-      <c r="H24" s="21"/>
-      <c r="I24" s="21"/>
-      <c r="J24" s="21"/>
-      <c r="K24" s="21"/>
-      <c r="L24" s="21"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="20"/>
+      <c r="L24" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="22">
@@ -5189,86 +5269,195 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5"/>
   <cols>
-    <col min="2" max="2" width="18.125" customWidth="1"/>
-    <col min="3" max="3" width="42.875" customWidth="1"/>
-    <col min="4" max="4" width="10.125" customWidth="1"/>
-    <col min="5" max="5" width="11.375" customWidth="1"/>
-    <col min="6" max="6" width="14.125" customWidth="1"/>
-    <col min="7" max="7" width="13.125" customWidth="1"/>
-    <col min="8" max="8" width="27.125" customWidth="1"/>
+    <col min="1" max="1" width="9.625" customWidth="1"/>
+    <col min="3" max="3" width="11.375" customWidth="1"/>
+    <col min="4" max="4" width="10.375" customWidth="1"/>
+    <col min="5" max="5" width="11.875" customWidth="1"/>
+    <col min="6" max="6" width="23" customWidth="1"/>
+    <col min="7" max="7" width="25.375" customWidth="1"/>
+    <col min="8" max="8" width="55.25" customWidth="1"/>
+    <col min="9" max="9" width="42.875" customWidth="1"/>
+    <col min="10" max="10" width="14.125" customWidth="1"/>
+    <col min="11" max="12" width="13.125" customWidth="1"/>
+    <col min="13" max="13" width="46" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="5" customFormat="1">
-      <c r="A1" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>21</v>
+    <row r="1" spans="1:13" s="5" customFormat="1">
+      <c r="A1" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>112</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="I1" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="J1" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="M1" s="12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
+    <row r="2" spans="1:13" ht="70.5" customHeight="1">
+      <c r="A2" s="27" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="G2" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="I2" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="K2" s="25">
+        <v>42578</v>
+      </c>
+      <c r="L2" s="25">
+        <v>42587</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>110</v>
+      </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
+    <row r="3" spans="1:13" ht="64.5" customHeight="1">
+      <c r="A3" s="27" t="s">
+        <v>136</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="G3" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="I3" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="K3" s="25">
+        <v>42578</v>
+      </c>
+      <c r="L3" s="25">
+        <v>42587</v>
+      </c>
+      <c r="M3" s="9" t="s">
+        <v>110</v>
+      </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
+    <row r="4" spans="1:13" ht="60" customHeight="1">
+      <c r="A4" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="G4" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="I4" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="K4" s="25">
+        <v>42580</v>
+      </c>
+      <c r="L4" s="25">
+        <v>42587</v>
+      </c>
+      <c r="M4" s="9"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:13">
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
@@ -5277,8 +5466,13 @@
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:13">
       <c r="A6" s="9"/>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
@@ -5287,8 +5481,13 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:13">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
@@ -5297,8 +5496,13 @@
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:13">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -5307,8 +5511,13 @@
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:13">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
@@ -5317,8 +5526,13 @@
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:13">
       <c r="A10" s="9"/>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
@@ -5327,8 +5541,13 @@
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:13">
       <c r="A11" s="9"/>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
@@ -5337,8 +5556,13 @@
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:13">
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
@@ -5347,8 +5571,13 @@
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:13">
       <c r="A13" s="9"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
@@ -5357,8 +5586,13 @@
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:13">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
@@ -5367,8 +5601,13 @@
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:13">
       <c r="A15" s="9"/>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
@@ -5377,8 +5616,13 @@
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:13">
       <c r="A16" s="9"/>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
@@ -5387,8 +5631,15 @@
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
+      <c r="I16" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:13">
       <c r="A17" s="9"/>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
@@ -5397,8 +5648,13 @@
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:13">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
@@ -5407,8 +5663,13 @@
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:13">
       <c r="A19" s="9"/>
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
@@ -5417,8 +5678,13 @@
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
       <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:13">
       <c r="A20" s="9"/>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
@@ -5427,10 +5693,20 @@
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
       <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>